<commit_message>
Revision by Oswaldo Garcia
</commit_message>
<xml_diff>
--- a/Doc/Window lifter/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/Doc/Window lifter/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isa\Dropbox\AEP - Continental\Mod_2_-_Ing_de_SW-2015-10-05\Window Lifter\V-Cycle Process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emma\Desktop\Repositorio Isa\trunk\Doc\Window lifter\V-Cycle Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="2"/>
+    <workbookView xWindow="7896" yWindow="3180" windowWidth="15012" windowHeight="9336" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1993,9 +1993,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2008,26 +2008,26 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" customWidth="1"/>
-    <col min="5" max="5" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.109375" customWidth="1"/>
+    <col min="5" max="5" width="84.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
@@ -2043,25 +2043,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:5" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="14"/>
       <c r="D9" s="40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:5" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="20"/>
       <c r="D10" s="41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="5"/>
       <c r="D11" s="42" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="10" t="s">
         <v>1</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="51">
         <v>1</v>
       </c>
@@ -2083,28 +2083,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="51"/>
       <c r="D15" s="52"/>
       <c r="E15" s="29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="31" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="51">
         <v>2</v>
       </c>
@@ -2115,33 +2115,33 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="51"/>
       <c r="D19" s="52"/>
       <c r="E19" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="51"/>
       <c r="D21" s="52"/>
       <c r="E21" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="51">
         <v>3</v>
       </c>
@@ -2152,28 +2152,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
       <c r="E24" s="35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
       <c r="E25" s="29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C28" s="16" t="s">
         <v>8</v>
       </c>
@@ -2181,31 +2181,31 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" s="17"/>
       <c r="D29" s="34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="3:5" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:5" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C30" s="36"/>
       <c r="D30" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="36"/>
       <c r="D31" s="34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" s="18"/>
       <c r="D32" s="26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="3:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="49"/>
       <c r="D33" s="50"/>
     </row>
@@ -2234,26 +2234,26 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="C2:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" customWidth="1"/>
-    <col min="5" max="5" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" customWidth="1"/>
+    <col min="5" max="5" width="84.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
@@ -2269,31 +2269,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="33"/>
       <c r="D9" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="33"/>
       <c r="D10" s="40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="33"/>
       <c r="D11" s="40" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="5"/>
       <c r="D12" s="46" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="10" t="s">
         <v>1</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="51">
         <v>1</v>
       </c>
@@ -2315,28 +2315,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="51">
         <v>2</v>
       </c>
@@ -2347,24 +2347,24 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="51"/>
       <c r="D21" s="52"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="7" t="s">
         <v>8</v>
       </c>
@@ -2372,19 +2372,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="11"/>
       <c r="D25" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="33"/>
       <c r="D26" s="30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
       <c r="D27" s="26" t="s">
         <v>98</v>
@@ -2412,26 +2412,26 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="C2:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="21"/>
-    <col min="3" max="3" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.5703125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="72.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="2" width="9.109375" style="21"/>
+    <col min="3" max="3" width="22.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="72.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="22"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
@@ -2447,31 +2447,31 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="33"/>
       <c r="D9" s="40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="33"/>
       <c r="D10" s="40" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="33"/>
       <c r="D11" s="40" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="26"/>
       <c r="D12" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="32" t="s">
         <v>1</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="51">
         <v>1</v>
       </c>
@@ -2493,26 +2493,26 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="31"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="51">
         <v>2</v>
       </c>
@@ -2523,26 +2523,26 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="51"/>
       <c r="D21" s="52"/>
       <c r="E21" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="51"/>
       <c r="D22" s="52"/>
       <c r="E22" s="26"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="51">
         <v>3</v>
       </c>
@@ -2553,26 +2553,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
       <c r="E24" s="37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
       <c r="E25" s="29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="26"/>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C28" s="28" t="s">
         <v>8</v>
       </c>
@@ -2580,19 +2580,19 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" s="33"/>
       <c r="D29" s="34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" s="33"/>
       <c r="D30" s="34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C31" s="26"/>
       <c r="D31" s="26" t="s">
         <v>98</v>
@@ -2629,24 +2629,24 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="21"/>
-    <col min="3" max="3" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.5703125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="72.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="2" width="9.109375" style="21"/>
+    <col min="3" max="3" width="22.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="72.44140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="22"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
@@ -2662,19 +2662,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="33"/>
       <c r="D9" s="29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="26"/>
       <c r="D10" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="32" t="s">
         <v>1</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="51">
         <v>1</v>
       </c>
@@ -2696,26 +2696,26 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="51"/>
       <c r="D14" s="52"/>
       <c r="E14" s="45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="51"/>
       <c r="D15" s="52"/>
       <c r="E15" s="30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="31"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="51">
         <v>2</v>
       </c>
@@ -2726,26 +2726,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C19" s="51"/>
       <c r="D19" s="52"/>
       <c r="E19" s="44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="31"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="28" t="s">
         <v>8</v>
       </c>
@@ -2753,19 +2753,19 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="33"/>
       <c r="D23" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="33"/>
       <c r="D24" s="29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="26"/>
       <c r="D25" s="26" t="s">
         <v>98</v>
@@ -2793,28 +2793,28 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="C2:E32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="21"/>
-    <col min="3" max="3" width="22.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.5703125" style="21" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="21"/>
+    <col min="3" max="3" width="22.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5546875" style="21" customWidth="1"/>
     <col min="5" max="5" width="82" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="21"/>
+    <col min="6" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="22"/>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="28" t="s">
         <v>3</v>
       </c>
@@ -2830,19 +2830,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="33"/>
       <c r="D9" s="29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="26"/>
       <c r="D10" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="32" t="s">
         <v>1</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="51">
         <v>1</v>
       </c>
@@ -2864,26 +2864,26 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="51"/>
       <c r="D14" s="52"/>
       <c r="E14" s="45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="51"/>
       <c r="D15" s="52"/>
       <c r="E15" s="30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="51"/>
       <c r="D16" s="52"/>
       <c r="E16" s="31"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="51">
         <v>2</v>
       </c>
@@ -2894,26 +2894,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C19" s="51"/>
       <c r="D19" s="52"/>
       <c r="E19" s="44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="51"/>
       <c r="D20" s="52"/>
       <c r="E20" s="31"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="28" t="s">
         <v>8</v>
       </c>
@@ -2921,34 +2921,34 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="33"/>
       <c r="D24" s="29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="33"/>
       <c r="D25" s="29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="33"/>
       <c r="D26" s="29" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C27" s="26"/>
       <c r="D27" s="26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D28" s="39"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" s="53"/>
       <c r="D29" s="52" t="s">
         <v>85</v>
@@ -2957,21 +2957,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" s="53"/>
       <c r="D30" s="52"/>
       <c r="E30" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C31" s="53"/>
       <c r="D31" s="52"/>
       <c r="E31" s="44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C32" s="53"/>
       <c r="D32" s="52"/>
       <c r="E32" s="43" t="s">

</xml_diff>